<commit_message>
push docs wijzigingen (timesheet, productiedossier, presentatie)
</commit_message>
<xml_diff>
--- a/docs/Timesheet_Joran_Vanhaste.xlsx
+++ b/docs/Timesheet_Joran_Vanhaste.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joran/Code/cmp3.local/docs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14920" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,9 +27,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Timesheet CMP III</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Taak</t>
+  </si>
+  <si>
+    <t>uur</t>
+  </si>
+  <si>
+    <t>sitemap+ productiedossier opstarten</t>
+  </si>
+  <si>
+    <t>Moodboard + style tiles</t>
+  </si>
+  <si>
+    <t>Style Tiles afwerken</t>
+  </si>
+  <si>
+    <t>Wireframes</t>
+  </si>
+  <si>
+    <t>Wireframes afwerken + visual designs</t>
+  </si>
+  <si>
+    <t>Visuals afwerken</t>
+  </si>
+  <si>
+    <t>productiedossier samenstellen en afwerken, alles pushen</t>
+  </si>
+  <si>
+    <t>contactformulier in drupal 7 toevoegen + logo en naam veranderen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">juiste mappenstructuur </t>
+  </si>
+  <si>
+    <t>Disclaimer + footer link+ Wijzigingen pushen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mappenstructuur gitlab aanpassen + repository gitlab </t>
   </si>
 </sst>
 </file>
@@ -34,7 +84,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -65,15 +114,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normaal" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -399,25 +459,165 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="23">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>42661</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>42663</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>42664</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>42666</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>42667</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>42668</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>42669</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>42672</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>42679</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>42681</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>42682</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <f>SUM(C3:C13)</f>
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>